<commit_message>
map term IRIs in BFO 2.0 Alan version to BFO 2.0 Graz version
</commit_message>
<xml_diff>
--- a/2012-01-05/doc/termsMapping.xlsx
+++ b/2012-01-05/doc/termsMapping.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="105" windowWidth="22815" windowHeight="11700"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="BFO1.1 to Alan to Graz" sheetId="4" r:id="rId1"/>
+    <sheet name="BFO1.1 to Alan Version" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="124">
   <si>
     <t>http://purl.org/obo/owl/OBO_REL#bearer_of</t>
   </si>
@@ -226,23 +227,173 @@
     <t>http://purl.obolibrary.org/obo/bfo/region-classes.owl</t>
   </si>
   <si>
-    <t>OBI terms: is concretization of</t>
-  </si>
-  <si>
-    <t>OBI terms: is concretization as</t>
-  </si>
-  <si>
     <t>OBI terms: is realized by</t>
   </si>
   <si>
     <t>OBI terms: realizes</t>
+  </si>
+  <si>
+    <t>BFO 1.1 and RO</t>
+  </si>
+  <si>
+    <t>BFO 2.0 Alan Version</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/BFO_0000015</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/BFO_0000176</t>
+  </si>
+  <si>
+    <t>part of continuant at some time</t>
+  </si>
+  <si>
+    <t>for continuant</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/BFO_0000132</t>
+  </si>
+  <si>
+    <t>part of occurrent</t>
+  </si>
+  <si>
+    <t>for occurrent</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/BFO_0000178</t>
+  </si>
+  <si>
+    <t>has continuant part at some time</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/BFO_0000117</t>
+  </si>
+  <si>
+    <t>has occurrent part</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/BFO_0000171</t>
+  </si>
+  <si>
+    <t>located in at some times</t>
+  </si>
+  <si>
+    <t>is 'located in at all times' in BFO 2.0 Graz version</t>
+  </si>
+  <si>
+    <t>participates in at some time</t>
+  </si>
+  <si>
+    <t>Labels in BFO 2.0 Graz</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>inheres in at all times</t>
+  </si>
+  <si>
+    <t>bearer of at some time</t>
+  </si>
+  <si>
+    <t>function of at all times</t>
+  </si>
+  <si>
+    <t>quality of at all times</t>
+  </si>
+  <si>
+    <t>role of at all times</t>
+  </si>
+  <si>
+    <t>entity</t>
+  </si>
+  <si>
+    <t>continuant</t>
+  </si>
+  <si>
+    <t>not in BFO 2.0 Graz version</t>
+  </si>
+  <si>
+    <t>disposition</t>
+  </si>
+  <si>
+    <t>function</t>
+  </si>
+  <si>
+    <t>generically dependent continuant</t>
+  </si>
+  <si>
+    <t>independent continuant</t>
+  </si>
+  <si>
+    <t>material entity</t>
+  </si>
+  <si>
+    <t>quality</t>
+  </si>
+  <si>
+    <t>realizable entity</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>site</t>
+  </si>
+  <si>
+    <t>specifically dependent continuant</t>
+  </si>
+  <si>
+    <t>process</t>
+  </si>
+  <si>
+    <t>occurrent</t>
+  </si>
+  <si>
+    <t>BFO 2.0 Graz different from BFO2.0 Alan</t>
+  </si>
+  <si>
+    <t>has participant at some time</t>
+  </si>
+  <si>
+    <t>zero-dimensional spatial region</t>
+  </si>
+  <si>
+    <t>one-dimensional spatial region</t>
+  </si>
+  <si>
+    <t>two-dimensional spatial region</t>
+  </si>
+  <si>
+    <t>three-dimensional spatial region</t>
+  </si>
+  <si>
+    <t>concretized by at some time</t>
+  </si>
+  <si>
+    <t>concretizes at some time</t>
+  </si>
+  <si>
+    <t>OBI terms: is_concretization_of</t>
+  </si>
+  <si>
+    <t>OBI terms: is_concretized_as</t>
+  </si>
+  <si>
+    <t>realizes</t>
+  </si>
+  <si>
+    <t>realized in</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -256,6 +407,14 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -282,12 +441,17 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -583,182 +747,782 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="103" customWidth="1"/>
+    <col min="1" max="1" width="65.42578125" customWidth="1"/>
+    <col min="2" max="2" width="42.5703125" customWidth="1"/>
+    <col min="3" max="3" width="49.7109375" customWidth="1"/>
+    <col min="4" max="4" width="41.42578125" customWidth="1"/>
+    <col min="5" max="5" width="30.5703125" customWidth="1"/>
+    <col min="6" max="6" width="33.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="5" customFormat="1" ht="15.75">
+      <c r="A1" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" t="s">
+        <v>99</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E21" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" t="s">
+        <v>99</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E22" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" t="s">
+        <v>99</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E24" t="s">
+        <v>83</v>
+      </c>
+      <c r="F24" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="D25" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E25" t="s">
+        <v>85</v>
+      </c>
+      <c r="F25" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" t="s">
+        <v>88</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E26" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" t="s">
+        <v>99</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E27" t="s">
+        <v>77</v>
+      </c>
+      <c r="F27" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="D28" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E28" t="s">
+        <v>80</v>
+      </c>
+      <c r="F28" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E31" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E32" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E33" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E34" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C35" t="s">
+        <v>121</v>
+      </c>
+      <c r="D35" s="2"/>
+      <c r="E35" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C36" t="s">
+        <v>120</v>
+      </c>
+      <c r="D36" s="2"/>
+      <c r="E36" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C37" t="s">
+        <v>70</v>
+      </c>
+      <c r="E37" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C38" t="s">
+        <v>71</v>
+      </c>
+      <c r="E38" t="s">
+        <v>122</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" location="function_of"/>
+    <hyperlink ref="A5" r:id="rId2" location="quality_of"/>
+    <hyperlink ref="A6" r:id="rId3" location="role_of"/>
+    <hyperlink ref="A26" r:id="rId4" location="located_in"/>
+    <hyperlink ref="A2" r:id="rId5" location="bearer_of"/>
+    <hyperlink ref="B2" r:id="rId6"/>
+    <hyperlink ref="A4" r:id="rId7" location="inheres_in"/>
+    <hyperlink ref="B4" r:id="rId8"/>
+    <hyperlink ref="A7" r:id="rId9" location="Entity"/>
+    <hyperlink ref="B7" r:id="rId10"/>
+    <hyperlink ref="A8" r:id="rId11" location="Continuant"/>
+    <hyperlink ref="B8" r:id="rId12"/>
+    <hyperlink ref="A9" r:id="rId13" location="DependentContinuant"/>
+    <hyperlink ref="B9" r:id="rId14"/>
+    <hyperlink ref="A10" r:id="rId15" location="Disposition"/>
+    <hyperlink ref="B10" r:id="rId16"/>
+    <hyperlink ref="A11" r:id="rId17" location="Function"/>
+    <hyperlink ref="B11" r:id="rId18"/>
+    <hyperlink ref="A12" r:id="rId19" location="GenericallyDependentContinuant"/>
+    <hyperlink ref="B12" r:id="rId20"/>
+    <hyperlink ref="A13" r:id="rId21" location="IndependentContinuant"/>
+    <hyperlink ref="B13" r:id="rId22"/>
+    <hyperlink ref="A14" r:id="rId23" location="MaterialEntity"/>
+    <hyperlink ref="B14" r:id="rId24"/>
+    <hyperlink ref="A15" r:id="rId25" location="Quality"/>
+    <hyperlink ref="B15" r:id="rId26"/>
+    <hyperlink ref="A16" r:id="rId27" location="RealizableEntity"/>
+    <hyperlink ref="B16" r:id="rId28"/>
+    <hyperlink ref="A17" r:id="rId29" location="Role"/>
+    <hyperlink ref="B17" r:id="rId30"/>
+    <hyperlink ref="A18" r:id="rId31" location="Site"/>
+    <hyperlink ref="B18" r:id="rId32"/>
+    <hyperlink ref="A19" r:id="rId33" location="SpecificallyDependentContinuant"/>
+    <hyperlink ref="B19" r:id="rId34"/>
+    <hyperlink ref="A34" r:id="rId35" location="ThreeDimensionalRegion"/>
+    <hyperlink ref="B34" r:id="rId36"/>
+    <hyperlink ref="A20" r:id="rId37" location="Occurrent"/>
+    <hyperlink ref="B20" r:id="rId38"/>
+    <hyperlink ref="A22" r:id="rId39" location="ProcessualEntity"/>
+    <hyperlink ref="B22" r:id="rId40"/>
+    <hyperlink ref="B24" r:id="rId41"/>
+    <hyperlink ref="B23" r:id="rId42"/>
+    <hyperlink ref="B27" r:id="rId43"/>
+    <hyperlink ref="B29" r:id="rId44"/>
+    <hyperlink ref="B30" r:id="rId45"/>
+    <hyperlink ref="A30" r:id="rId46" location="preceded_by"/>
+    <hyperlink ref="A29" r:id="rId47" location="participates_in"/>
+    <hyperlink ref="A27" r:id="rId48" location="part_of"/>
+    <hyperlink ref="A23" r:id="rId49" location="has_participant"/>
+    <hyperlink ref="A24" r:id="rId50" location="has_part"/>
+    <hyperlink ref="B3" r:id="rId51"/>
+    <hyperlink ref="B5" r:id="rId52"/>
+    <hyperlink ref="B6" r:id="rId53"/>
+    <hyperlink ref="B26" r:id="rId54"/>
+    <hyperlink ref="A35" r:id="rId55"/>
+    <hyperlink ref="A36" r:id="rId56"/>
+    <hyperlink ref="A37" r:id="rId57"/>
+    <hyperlink ref="B37" r:id="rId58"/>
+    <hyperlink ref="B35" r:id="rId59"/>
+    <hyperlink ref="B36" r:id="rId60"/>
+    <hyperlink ref="B38" r:id="rId61"/>
+    <hyperlink ref="A38" r:id="rId62"/>
+    <hyperlink ref="A21" r:id="rId63" location="Process"/>
+    <hyperlink ref="B21" r:id="rId64"/>
+    <hyperlink ref="A32" r:id="rId65" location="OneDimensionalRegion"/>
+    <hyperlink ref="A33" r:id="rId66" location="TwoDimensionalRegion"/>
+    <hyperlink ref="A31" r:id="rId67" location="ZeroDimensionalRegion"/>
+    <hyperlink ref="B31" r:id="rId68"/>
+    <hyperlink ref="B32" r:id="rId69"/>
+    <hyperlink ref="B33" r:id="rId70"/>
+    <hyperlink ref="C34" r:id="rId71"/>
+    <hyperlink ref="C33" r:id="rId72"/>
+    <hyperlink ref="C32" r:id="rId73"/>
+    <hyperlink ref="C31" r:id="rId74"/>
+    <hyperlink ref="D21" r:id="rId75"/>
+    <hyperlink ref="D22" r:id="rId76"/>
+    <hyperlink ref="D27" r:id="rId77"/>
+    <hyperlink ref="D28" r:id="rId78"/>
+    <hyperlink ref="D24" r:id="rId79"/>
+    <hyperlink ref="D25" r:id="rId80"/>
+    <hyperlink ref="D26" r:id="rId81"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId82"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C36"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C34" sqref="C33:C34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="75.5703125" customWidth="1"/>
     <col min="2" max="2" width="47.42578125" customWidth="1"/>
     <col min="3" max="3" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
+      <c r="A1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="1" t="s">
-        <v>62</v>
+        <v>37</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>20</v>
@@ -766,69 +1530,66 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="1" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="1" t="s">
-        <v>43</v>
+        <v>1</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="1" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="1" t="s">
-        <v>65</v>
+        <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>69</v>
@@ -836,10 +1597,10 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>69</v>
@@ -847,24 +1608,24 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>18</v>
+        <v>64</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C32" t="s">
-        <v>70</v>
+      <c r="A32" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -872,32 +1633,43 @@
         <v>35</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C33" t="s">
-        <v>71</v>
+        <v>121</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C34" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B35" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C34" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="1" t="s">
+      <c r="C35" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C35" t="s">
-        <v>73</v>
+      <c r="C36" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -905,80 +1677,80 @@
     <sortCondition ref="A1:A27"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" location="function_of"/>
-    <hyperlink ref="A4" r:id="rId2" location="quality_of"/>
-    <hyperlink ref="A5" r:id="rId3" location="role_of"/>
-    <hyperlink ref="A24" r:id="rId4" location="located_in"/>
-    <hyperlink ref="A1" r:id="rId5" location="bearer_of"/>
-    <hyperlink ref="B1" r:id="rId6"/>
-    <hyperlink ref="A3" r:id="rId7" location="inheres_in"/>
-    <hyperlink ref="B3" r:id="rId8"/>
-    <hyperlink ref="A6" r:id="rId9" location="Entity"/>
-    <hyperlink ref="B6" r:id="rId10"/>
-    <hyperlink ref="A7" r:id="rId11" location="Continuant"/>
-    <hyperlink ref="B7" r:id="rId12"/>
-    <hyperlink ref="A8" r:id="rId13" location="DependentContinuant"/>
-    <hyperlink ref="B8" r:id="rId14"/>
-    <hyperlink ref="A9" r:id="rId15" location="Disposition"/>
-    <hyperlink ref="B9" r:id="rId16"/>
-    <hyperlink ref="A10" r:id="rId17" location="Function"/>
-    <hyperlink ref="B10" r:id="rId18"/>
-    <hyperlink ref="A11" r:id="rId19" location="GenericallyDependentContinuant"/>
-    <hyperlink ref="B11" r:id="rId20"/>
-    <hyperlink ref="A12" r:id="rId21" location="IndependentContinuant"/>
-    <hyperlink ref="B12" r:id="rId22"/>
-    <hyperlink ref="A13" r:id="rId23" location="MaterialEntity"/>
-    <hyperlink ref="B13" r:id="rId24"/>
-    <hyperlink ref="A14" r:id="rId25" location="Quality"/>
-    <hyperlink ref="B14" r:id="rId26"/>
-    <hyperlink ref="A15" r:id="rId27" location="RealizableEntity"/>
-    <hyperlink ref="B15" r:id="rId28"/>
-    <hyperlink ref="A16" r:id="rId29" location="Role"/>
-    <hyperlink ref="B16" r:id="rId30"/>
-    <hyperlink ref="A17" r:id="rId31" location="Site"/>
-    <hyperlink ref="B17" r:id="rId32"/>
-    <hyperlink ref="A18" r:id="rId33" location="SpecificallyDependentContinuant"/>
-    <hyperlink ref="B18" r:id="rId34"/>
-    <hyperlink ref="A31" r:id="rId35" location="ThreeDimensionalRegion"/>
-    <hyperlink ref="B31" r:id="rId36"/>
-    <hyperlink ref="A19" r:id="rId37" location="Occurrent"/>
-    <hyperlink ref="B19" r:id="rId38"/>
-    <hyperlink ref="A21" r:id="rId39" location="ProcessualEntity"/>
-    <hyperlink ref="B21" r:id="rId40"/>
-    <hyperlink ref="B23" r:id="rId41"/>
-    <hyperlink ref="B22" r:id="rId42"/>
-    <hyperlink ref="B25" r:id="rId43"/>
-    <hyperlink ref="B26" r:id="rId44"/>
-    <hyperlink ref="B27" r:id="rId45"/>
-    <hyperlink ref="A27" r:id="rId46" location="preceded_by"/>
-    <hyperlink ref="A26" r:id="rId47" location="participates_in"/>
-    <hyperlink ref="A25" r:id="rId48" location="part_of"/>
-    <hyperlink ref="A22" r:id="rId49" location="has_participant"/>
-    <hyperlink ref="A23" r:id="rId50" location="has_part"/>
-    <hyperlink ref="B2" r:id="rId51"/>
-    <hyperlink ref="B4" r:id="rId52"/>
-    <hyperlink ref="B5" r:id="rId53"/>
-    <hyperlink ref="B24" r:id="rId54"/>
-    <hyperlink ref="A32" r:id="rId55"/>
-    <hyperlink ref="A33" r:id="rId56"/>
-    <hyperlink ref="A34" r:id="rId57"/>
+    <hyperlink ref="A3" r:id="rId1" location="function_of"/>
+    <hyperlink ref="A5" r:id="rId2" location="quality_of"/>
+    <hyperlink ref="A6" r:id="rId3" location="role_of"/>
+    <hyperlink ref="A25" r:id="rId4" location="located_in"/>
+    <hyperlink ref="A2" r:id="rId5" location="bearer_of"/>
+    <hyperlink ref="B2" r:id="rId6"/>
+    <hyperlink ref="A4" r:id="rId7" location="inheres_in"/>
+    <hyperlink ref="B4" r:id="rId8"/>
+    <hyperlink ref="A7" r:id="rId9" location="Entity"/>
+    <hyperlink ref="B7" r:id="rId10"/>
+    <hyperlink ref="A8" r:id="rId11" location="Continuant"/>
+    <hyperlink ref="B8" r:id="rId12"/>
+    <hyperlink ref="A9" r:id="rId13" location="DependentContinuant"/>
+    <hyperlink ref="B9" r:id="rId14"/>
+    <hyperlink ref="A10" r:id="rId15" location="Disposition"/>
+    <hyperlink ref="B10" r:id="rId16"/>
+    <hyperlink ref="A11" r:id="rId17" location="Function"/>
+    <hyperlink ref="B11" r:id="rId18"/>
+    <hyperlink ref="A12" r:id="rId19" location="GenericallyDependentContinuant"/>
+    <hyperlink ref="B12" r:id="rId20"/>
+    <hyperlink ref="A13" r:id="rId21" location="IndependentContinuant"/>
+    <hyperlink ref="B13" r:id="rId22"/>
+    <hyperlink ref="A14" r:id="rId23" location="MaterialEntity"/>
+    <hyperlink ref="B14" r:id="rId24"/>
+    <hyperlink ref="A15" r:id="rId25" location="Quality"/>
+    <hyperlink ref="B15" r:id="rId26"/>
+    <hyperlink ref="A16" r:id="rId27" location="RealizableEntity"/>
+    <hyperlink ref="B16" r:id="rId28"/>
+    <hyperlink ref="A17" r:id="rId29" location="Role"/>
+    <hyperlink ref="B17" r:id="rId30"/>
+    <hyperlink ref="A18" r:id="rId31" location="Site"/>
+    <hyperlink ref="B18" r:id="rId32"/>
+    <hyperlink ref="A19" r:id="rId33" location="SpecificallyDependentContinuant"/>
+    <hyperlink ref="B19" r:id="rId34"/>
+    <hyperlink ref="A32" r:id="rId35" location="ThreeDimensionalRegion"/>
+    <hyperlink ref="B32" r:id="rId36"/>
+    <hyperlink ref="A20" r:id="rId37" location="Occurrent"/>
+    <hyperlink ref="B20" r:id="rId38"/>
+    <hyperlink ref="A22" r:id="rId39" location="ProcessualEntity"/>
+    <hyperlink ref="B22" r:id="rId40"/>
+    <hyperlink ref="B24" r:id="rId41"/>
+    <hyperlink ref="B23" r:id="rId42"/>
+    <hyperlink ref="B26" r:id="rId43"/>
+    <hyperlink ref="B27" r:id="rId44"/>
+    <hyperlink ref="B28" r:id="rId45"/>
+    <hyperlink ref="A28" r:id="rId46" location="preceded_by"/>
+    <hyperlink ref="A27" r:id="rId47" location="participates_in"/>
+    <hyperlink ref="A26" r:id="rId48" location="part_of"/>
+    <hyperlink ref="A23" r:id="rId49" location="has_participant"/>
+    <hyperlink ref="A24" r:id="rId50" location="has_part"/>
+    <hyperlink ref="B3" r:id="rId51"/>
+    <hyperlink ref="B5" r:id="rId52"/>
+    <hyperlink ref="B6" r:id="rId53"/>
+    <hyperlink ref="B25" r:id="rId54"/>
+    <hyperlink ref="A35" r:id="rId55"/>
+    <hyperlink ref="B35" r:id="rId56"/>
+    <hyperlink ref="B33" r:id="rId57"/>
     <hyperlink ref="B34" r:id="rId58"/>
-    <hyperlink ref="B32" r:id="rId59"/>
-    <hyperlink ref="B33" r:id="rId60"/>
-    <hyperlink ref="B35" r:id="rId61"/>
-    <hyperlink ref="A35" r:id="rId62"/>
-    <hyperlink ref="A20" r:id="rId63" location="Process"/>
-    <hyperlink ref="B20" r:id="rId64"/>
-    <hyperlink ref="A29" r:id="rId65" location="OneDimensionalRegion"/>
-    <hyperlink ref="A30" r:id="rId66" location="TwoDimensionalRegion"/>
-    <hyperlink ref="A28" r:id="rId67" location="ZeroDimensionalRegion"/>
-    <hyperlink ref="B28" r:id="rId68"/>
-    <hyperlink ref="B29" r:id="rId69"/>
-    <hyperlink ref="B30" r:id="rId70"/>
-    <hyperlink ref="C31" r:id="rId71"/>
-    <hyperlink ref="C30" r:id="rId72"/>
-    <hyperlink ref="C29" r:id="rId73"/>
-    <hyperlink ref="C28" r:id="rId74"/>
+    <hyperlink ref="B36" r:id="rId59"/>
+    <hyperlink ref="A36" r:id="rId60"/>
+    <hyperlink ref="A21" r:id="rId61" location="Process"/>
+    <hyperlink ref="B21" r:id="rId62"/>
+    <hyperlink ref="A30" r:id="rId63" location="OneDimensionalRegion"/>
+    <hyperlink ref="A31" r:id="rId64" location="TwoDimensionalRegion"/>
+    <hyperlink ref="A29" r:id="rId65" location="ZeroDimensionalRegion"/>
+    <hyperlink ref="B29" r:id="rId66"/>
+    <hyperlink ref="B30" r:id="rId67"/>
+    <hyperlink ref="B31" r:id="rId68"/>
+    <hyperlink ref="C32" r:id="rId69"/>
+    <hyperlink ref="C31" r:id="rId70"/>
+    <hyperlink ref="C30" r:id="rId71"/>
+    <hyperlink ref="C29" r:id="rId72"/>
+    <hyperlink ref="A33" r:id="rId73"/>
+    <hyperlink ref="A34" r:id="rId74"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId75"/>

</xml_diff>